<commit_message>
Auto-committed on 2022/04/29 週五
</commit_message>
<xml_diff>
--- a/Program/Other/L9730_定期機動資料檢核.xlsx
+++ b/Program/Other/L9730_定期機動資料檢核.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A8F90B-125D-421A-90DF-1F7D74E87F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569A45A8-7E0D-4FA5-BE2F-3287531321EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="252" yWindow="408" windowWidth="22788" windowHeight="11952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="X800" sheetId="2" r:id="rId1"/>
@@ -25,43 +25,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>LMSACN</t>
+    <t>戶號</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LMSAPN</t>
+    <t>額度</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LMSASQ</t>
+    <t>撥款序號</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LMSNSD</t>
+    <t>基本利率代碼</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LMSFSD</t>
+    <t>利率加減碼</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>IRTBCD</t>
+    <t>加碼生效日期</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>IRTASC</t>
+    <t>加碼利率</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ASCADT</t>
+    <t>放款餘額</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ASCRAT</t>
+    <t>下次調息日期</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LMSLBL</t>
+    <t>首次調息日期</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1057,12 +1057,12 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1077,25 +1077,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/03 週二
</commit_message>
<xml_diff>
--- a/Program/Other/L9730_定期機動資料檢核.xlsx
+++ b/Program/Other/L9730_定期機動資料檢核.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569A45A8-7E0D-4FA5-BE2F-3287531321EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE5CC21-D81F-43EE-82ED-C5C07E543A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="408" windowWidth="22788" windowHeight="11952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="X800" sheetId="2" r:id="rId1"/>
@@ -37,10 +37,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>基本利率代碼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>利率加減碼</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -57,11 +53,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>下次調息日期</t>
+    <t>下次調整日期</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>首次調息日期</t>
+    <t>首次調整日期</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品代碼</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1077,25 +1077,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>